<commit_message>
Supplier risk update part1
CRQ for Cyber Days 2024
</commit_message>
<xml_diff>
--- a/XLS-spreadsheets/EN Ransomware Mitigation Using EDR and SOC.xlsx
+++ b/XLS-spreadsheets/EN Ransomware Mitigation Using EDR and SOC.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad3d434324f7e88d/Documents/CyberRangers/Cyb3r Days 2022/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ad3d434324f7e88d/Documents/GitHub/CRQ/XLS-spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="36" documentId="8_{0DC40DCD-585B-4503-A2F6-4975B6057617}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{337123F8-D748-401C-A5F4-84F73201417E}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1837" windowWidth="21480" windowHeight="11663" xr2:uid="{E98B0EBF-165E-4020-AC73-88DAD624F08B}"/>
+    <workbookView xWindow="435" yWindow="45" windowWidth="21165" windowHeight="12735" xr2:uid="{E98B0EBF-165E-4020-AC73-88DAD624F08B}"/>
   </bookViews>
   <sheets>
     <sheet name="EDR and SOC" sheetId="1" r:id="rId1"/>
@@ -537,11 +537,11 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -863,8 +863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C867A4A-84E6-4930-A215-1CD45A6AE281}">
   <dimension ref="A2:H95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77"/>
+    <sheetView tabSelected="1" topLeftCell="B62" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1057,7 +1057,7 @@
       <c r="F28" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="18">
+      <c r="G28" s="17">
         <f>C28*(1-E28)</f>
         <v>2.2499999999999998E-3</v>
       </c>
@@ -1081,7 +1081,7 @@
       <c r="F29" t="s">
         <v>2</v>
       </c>
-      <c r="G29" s="18">
+      <c r="G29" s="17">
         <f>C29*(1-E29)</f>
         <v>9.3750000000000018E-4</v>
       </c>
@@ -1105,7 +1105,7 @@
       <c r="F30" t="s">
         <v>2</v>
       </c>
-      <c r="G30" s="18">
+      <c r="G30" s="17">
         <f>C30*(1-E30)</f>
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1120,13 +1120,13 @@
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B32" s="17"/>
-      <c r="C32" s="17"/>
-      <c r="D32" s="17"/>
-      <c r="E32" s="17"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="19"/>
+      <c r="D32" s="19"/>
+      <c r="E32" s="19"/>
       <c r="G32" s="3">
         <f>G31/$C$22</f>
         <v>0.62749999999999995</v>
@@ -1210,7 +1210,7 @@
       <c r="F43" t="s">
         <v>2</v>
       </c>
-      <c r="G43" s="18">
+      <c r="G43" s="17">
         <f>C43*(1-E43)</f>
         <v>1.1250000000000012E-4</v>
       </c>
@@ -1234,7 +1234,7 @@
       <c r="F44" t="s">
         <v>2</v>
       </c>
-      <c r="G44" s="18">
+      <c r="G44" s="17">
         <f>C44*(1-E44)</f>
         <v>0</v>
       </c>
@@ -1258,7 +1258,7 @@
       <c r="F45" t="s">
         <v>2</v>
       </c>
-      <c r="G45" s="18">
+      <c r="G45" s="17">
         <f>C45*(1-E45)</f>
         <v>1.1250000000000001E-2</v>
       </c>
@@ -1273,13 +1273,13 @@
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="B47" s="17"/>
-      <c r="C47" s="17"/>
-      <c r="D47" s="17"/>
-      <c r="E47" s="17"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
       <c r="G47" s="3">
         <f>G46/$C$22</f>
         <v>0.45450000000000002</v>
@@ -1363,7 +1363,7 @@
       <c r="F57" t="s">
         <v>4</v>
       </c>
-      <c r="G57" s="18">
+      <c r="G57" s="17">
         <f>C57*(1-E57)</f>
         <v>2.2499999999999998E-3</v>
       </c>
@@ -1387,7 +1387,7 @@
       <c r="F58" t="s">
         <v>4</v>
       </c>
-      <c r="G58" s="18">
+      <c r="G58" s="17">
         <f>C58*(1-E58)</f>
         <v>9.3750000000000018E-4</v>
       </c>
@@ -1411,7 +1411,7 @@
       <c r="F59" t="s">
         <v>4</v>
       </c>
-      <c r="G59" s="18">
+      <c r="G59" s="17">
         <f>C59*(1-E59)</f>
         <v>1.2500000000000001E-2</v>
       </c>
@@ -1436,7 +1436,7 @@
       <c r="F60" t="s">
         <v>5</v>
       </c>
-      <c r="G60" s="18">
+      <c r="G60" s="17">
         <f t="shared" ref="G60:G62" si="0">C60*(1-E60)</f>
         <v>2.2500000000000018E-5</v>
       </c>
@@ -1461,7 +1461,7 @@
       <c r="F61" t="s">
         <v>5</v>
       </c>
-      <c r="G61" s="18">
+      <c r="G61" s="17">
         <f t="shared" si="0"/>
         <v>9.3750000000000093E-6</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="F62" t="s">
         <v>5</v>
       </c>
-      <c r="G62" s="18">
+      <c r="G62" s="17">
         <f t="shared" si="0"/>
         <v>6.2500000000000003E-3</v>
       </c>
@@ -1599,7 +1599,7 @@
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F75" s="19">
+      <c r="F75" s="18">
         <v>0.30970101044634823</v>
       </c>
       <c r="G75" s="14" t="s">
@@ -1864,7 +1864,7 @@
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="F95" s="19">
+      <c r="F95" s="18">
         <v>1.3070769769392063</v>
       </c>
       <c r="G95" s="14" t="s">

</xml_diff>